<commit_message>
take weekends and non-working hours into account
</commit_message>
<xml_diff>
--- a/data/tek_data/GHD_Zonierung.xlsx
+++ b/data/tek_data/GHD_Zonierung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Verwaltungsgebäude" sheetId="1" r:id="rId1"/>
@@ -4878,8 +4878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4959,7 +4959,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="F3" s="59">
         <v>1</v>
@@ -5019,8 +5019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5100,7 +5100,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>52</v>
       </c>
       <c r="F3" s="59">
         <v>1</v>

</xml_diff>